<commit_message>
Unsupervised clustering, padding experiments
</commit_message>
<xml_diff>
--- a/model_metrics.xlsx
+++ b/model_metrics.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="rankings" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="rank" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="169">
   <si>
     <t xml:space="preserve">nb</t>
   </si>
@@ -180,10 +181,7 @@
     <t xml:space="preserve">03_7</t>
   </si>
   <si>
-    <t xml:space="preserve">wrong one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TODO Submit during the week (submission created)</t>
+    <t xml:space="preserve">Resnet 101, fp16 otherwise default transforms as 03_1</t>
   </si>
   <si>
     <t xml:space="preserve">stage-2-rn101-03_7-cv_reflect_101-20191031-5e1dab49</t>
@@ -219,6 +217,51 @@
     <t xml:space="preserve">qualitative testing of effect of stepping up image sizes, TODO more experiments</t>
   </si>
   <si>
+    <t xml:space="preserve">03_10_fastai_train_resnet_swa_20191104.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_11_fastai_train_resnet_valid_20191108.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As 03_1 valid only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_12_fastai_train_resnet_valid_cf_verified_20191108.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">predicted unverified and saved to csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_13_fastai_train_resnet_radam_20191108.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As 03_1 but with radm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_14_fastai_train_resnet_ranger_20191108.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO: created sub file, submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As 03_1 but with ranger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_15_fastai_train_resnet_valid_cf_verified_cutoff_20191109.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used predictions on test, invalid, looked at confidence histograms, use high confidence ones as part of trainign set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_18</t>
+  </si>
+  <si>
     <t xml:space="preserve">Using sharpend images</t>
   </si>
   <si>
@@ -279,6 +322,39 @@
     <t xml:space="preserve">Using data with border_reflect_101 and imgaug to add classes</t>
   </si>
   <si>
+    <t xml:space="preserve">Overfitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05_5_fastai_train_resnet_20191108.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imgaug of valid data only, adding 1000 imgaug images to each class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05_6_fastai_train_resnet_imgaug_pred_unverified_20191108.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imgaug of valid data + unverified that we predict to have the same class using 03_11 model, adding 1000 imgaug images to each class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05_7_fastai_train_resnet_minimal-imgaug_pred_unverified_20191108.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imgaug of valid data + unverified that we predict to have the same class using 03_11 model, adding imgaug images (exacty same as number in verified) to each class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05_8_fastai_train_resnet_miniminimal-imgaug_pred_unverified_20191108.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imgaug based on class level/4 + unverified that we predict to have the same class using 03_11 model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05_9_fastai_train_resnet_miniminimal-imgaug_pred_unverified_pred_test_20191109.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">using  predicted test with cutoffs and imgs aug class number/10 for training</t>
+  </si>
+  <si>
     <t xml:space="preserve">TODO – inference on 05_4 and 05_2, error on loading leading learnier rel to fp16</t>
   </si>
   <si>
@@ -345,6 +421,12 @@
     <t xml:space="preserve">created submission, todo: submit</t>
   </si>
   <si>
+    <t xml:space="preserve">06_8_fastai_train_wideresnet_20191107.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strted looking at this buty fair bit of work to get training then more work to get pred</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ensembles</t>
   </si>
   <si>
@@ -354,6 +436,24 @@
     <t xml:space="preserve">Simple ensemble using averaging of 2 x resnet, 1x densenet, 1x eficientnet</t>
   </si>
   <si>
+    <t xml:space="preserve">Unsupervised clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2d_clustering-train_valid.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08_1_clustering_qc_20191109.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustering detailed QC, nothing major stands </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
     <t xml:space="preserve">07_2</t>
   </si>
   <si>
@@ -366,12 +466,18 @@
     <t xml:space="preserve">reflect</t>
   </si>
   <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
     <t xml:space="preserve">basic transforms</t>
   </si>
   <si>
     <t xml:space="preserve">wrap</t>
   </si>
   <si>
+    <t xml:space="preserve">Resnet101</t>
+  </si>
+  <si>
     <t xml:space="preserve">imgaug</t>
   </si>
   <si>
@@ -391,6 +497,39 @@
   </si>
   <si>
     <t xml:space="preserve">06_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.kaggle.com/c/aptos2019-blindness-detection/discussion/108065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contrast_range=0.2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brightness_range=20.,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hue_range=10.,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saturation_range=20.,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blur_and_sharpen=True,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate_range=180.,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scale_range=0.2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shear_range=0.2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shift_range=0.2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do_mirror=True,</t>
   </si>
 </sst>
 </file>
@@ -400,7 +539,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -442,12 +581,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,7 +632,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8AA97"/>
-        <bgColor rgb="FFF68E76"/>
+        <bgColor rgb="FFFDC578"/>
       </patternFill>
     </fill>
     <fill>
@@ -516,8 +661,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFDC578"/>
+        <bgColor rgb="FFFFDAA2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC2E0AE"/>
         <bgColor rgb="FFBEE3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87D1D1"/>
+        <bgColor rgb="FF8CCFB7"/>
       </patternFill>
     </fill>
     <fill>
@@ -534,14 +691,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFADD58A"/>
-        <bgColor rgb="FFC2E0AE"/>
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF87D1D1"/>
-        <bgColor rgb="FF8CCFB7"/>
+        <fgColor rgb="FFADD58A"/>
+        <bgColor rgb="FFC2E0AE"/>
       </patternFill>
     </fill>
     <fill>
@@ -591,7 +748,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -652,15 +809,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -676,47 +841,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -724,7 +893,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -744,7 +913,7 @@
       <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -782,7 +951,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF87D1D1"/>
       <rgbColor rgb="FF72BF44"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFDC578"/>
       <rgbColor rgb="FFF68E76"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -833,6 +1002,8 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -842,10 +1013,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>rankings!$A$3:$A$13</c:f>
+              <c:f>rankings!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -878,16 +1049,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>rankings!$C$3:$C$13</c:f>
+              <c:f>rankings!$C$3:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.4306</c:v>
                 </c:pt>
@@ -898,27 +1072,30 @@
                   <c:v>0.4531</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.4849</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.489</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4947</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.4988</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.5043</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.5215</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.5543</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.5557</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.6312</c:v>
                 </c:pt>
               </c:numCache>
@@ -926,17 +1103,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9174256"/>
-        <c:axId val="26752398"/>
+        <c:axId val="9835685"/>
+        <c:axId val="48529175"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9174256"/>
+        <c:axId val="9835685"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -958,12 +1135,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26752398"/>
+        <c:crossAx val="48529175"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26752398"/>
+        <c:axId val="48529175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -978,7 +1155,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1000,7 +1177,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9174256"/>
+        <c:crossAx val="9835685"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1071,6 +1248,8 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1080,9 +1259,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>rankings!$A$3:$A$13</c:f>
+              <c:f>rankings!$A$3:$A$14</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>07_2</c:v>
                 </c:pt>
@@ -1093,27 +1272,30 @@
                   <c:v>05_3</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>03_7</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>05_2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>06_7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>03_8_3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>06_7_1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>03_8_1</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>06_3</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>05_4</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>06_6</c:v>
                 </c:pt>
               </c:strCache>
@@ -1121,10 +1303,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>rankings!$C$3:$C$13</c:f>
+              <c:f>rankings!$C$3:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.4306</c:v>
                 </c:pt>
@@ -1135,27 +1317,30 @@
                   <c:v>0.4531</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.4849</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.489</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4947</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.4988</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.5043</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.5215</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.5543</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.5557</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.6312</c:v>
                 </c:pt>
               </c:numCache>
@@ -1164,11 +1349,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="30408828"/>
-        <c:axId val="4305455"/>
+        <c:axId val="22864067"/>
+        <c:axId val="91927152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="30408828"/>
+        <c:axId val="22864067"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,14 +1381,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4305455"/>
+        <c:crossAx val="91927152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4305455"/>
+        <c:axId val="91927152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1218,7 +1403,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1240,7 +1425,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30408828"/>
+        <c:crossAx val="22864067"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1378,11 +1563,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="19927720"/>
-        <c:axId val="89665056"/>
+        <c:axId val="93109884"/>
+        <c:axId val="71181858"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19927720"/>
+        <c:axId val="93109884"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,14 +1595,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89665056"/>
+        <c:crossAx val="71181858"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89665056"/>
+        <c:axId val="71181858"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -1455,7 +1640,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19927720"/>
+        <c:crossAx val="93109884"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1507,16 +1692,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>783360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>783720</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>45360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>40680</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>38880</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>32040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1524,8 +1709,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9052920" y="2483640"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="9865800" y="2483640"/>
+        <a:ext cx="5757840" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1543,10 +1728,10 @@
       <xdr:rowOff>133920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>301680</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>300240</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1555,7 +1740,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="118800" y="2572200"/>
-        <a:ext cx="8452440" cy="3241800"/>
+        <a:ext cx="9263520" cy="3240000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1579,9 +1764,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>158040</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1590,7 +1775,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1714680" y="2696400"/>
-        <a:ext cx="5758560" cy="3241440"/>
+        <a:ext cx="5756760" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1608,28 +1793,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y66"/>
+  <dimension ref="A1:Y102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W66" activeCellId="0" sqref="W66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W39" activeCellId="0" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="2.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="2.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="3.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="34.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="59.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2008,14 +2190,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+    <row r="15" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="2" t="s">
         <v>51</v>
       </c>
       <c r="J15" s="9" t="n">
@@ -2045,22 +2228,22 @@
       <c r="R15" s="9" t="n">
         <v>0.131707</v>
       </c>
-      <c r="U15" s="15" t="n">
-        <v>12</v>
-      </c>
-      <c r="V15" s="16" t="s">
+      <c r="U15" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="V15" s="9" t="n">
+        <v>0.4849</v>
+      </c>
+      <c r="W15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="W15" s="15" t="s">
+      <c r="X15" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="X15" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
@@ -2077,7 +2260,7 @@
       <c r="R17" s="9" t="n">
         <v>0.129047</v>
       </c>
-      <c r="S17" s="17" t="n">
+      <c r="S17" s="15" t="n">
         <f aca="false">Q17/V17</f>
         <v>0.74729242569511</v>
       </c>
@@ -2091,7 +2274,7 @@
         <v>0.5215</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2099,7 +2282,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
@@ -2108,7 +2291,7 @@
         <v>20191102</v>
       </c>
       <c r="W19" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,19 +2299,19 @@
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" s="9" t="n">
         <v>20191102</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P21" s="9" t="n">
         <v>0.132052</v>
@@ -2153,7 +2336,7 @@
         <v>0.4988</v>
       </c>
       <c r="W21" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,616 +2344,952 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="W23" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="W23" s="15" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="9" t="n">
+        <v>0.460921</v>
+      </c>
+      <c r="K27" s="17" t="n">
+        <v>0.493934</v>
+      </c>
+      <c r="L27" s="9" t="n">
+        <v>0.184936</v>
+      </c>
+      <c r="U27" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="V27" s="0" t="n">
+        <v>0.4687</v>
+      </c>
+      <c r="W27" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="2" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="W29" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="V31" s="9" t="n">
+        <v>0.4521</v>
+      </c>
+      <c r="W31" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="V33" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="W33" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V34" s="19"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="W35" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="V37" s="0" t="n">
+        <v>0.5374</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="V38" s="0" t="n">
+        <v>0.5266</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="V39" s="0" t="n">
+        <v>0.4535</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="3" t="n">
+      <c r="D43" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="3" t="n">
         <v>20191027</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="0" t="n">
+      <c r="G43" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H43" s="0" t="n">
         <v>256</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I43" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="9" t="n">
+      <c r="J43" s="9" t="n">
         <v>0.371694</v>
       </c>
-      <c r="K27" s="18" t="n">
+      <c r="K43" s="20" t="n">
         <v>0.366708</v>
       </c>
-      <c r="L27" s="9" t="n">
+      <c r="L43" s="9" t="n">
         <v>0.129712</v>
       </c>
-      <c r="M27" s="9" t="n">
+      <c r="M43" s="9" t="n">
         <v>0.351872</v>
       </c>
-      <c r="N27" s="19" t="n">
+      <c r="N43" s="21" t="n">
         <v>0.355532</v>
       </c>
-      <c r="O27" s="9" t="n">
+      <c r="O43" s="9" t="n">
         <v>0.127273</v>
       </c>
-      <c r="W27" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="U43" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="V43" s="9" t="n">
+        <v>0.4916</v>
+      </c>
+      <c r="W43" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" s="3" t="n">
+        <v>20191028</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="J48" s="9" t="n">
+        <v>0.322902</v>
+      </c>
+      <c r="K48" s="22" t="n">
+        <v>0.375154</v>
+      </c>
+      <c r="L48" s="9" t="n">
+        <v>0.144468</v>
+      </c>
+      <c r="M48" s="9" t="n">
+        <v>0.299865</v>
+      </c>
+      <c r="N48" s="23" t="n">
+        <v>0.334215</v>
+      </c>
+      <c r="O48" s="9" t="n">
+        <v>0.128337</v>
+      </c>
+      <c r="P48" s="9" t="n">
+        <v>0.265335</v>
+      </c>
+      <c r="Q48" s="9" t="n">
+        <v>0.325966</v>
+      </c>
+      <c r="R48" s="9" t="n">
+        <v>0.124625</v>
+      </c>
+      <c r="S48" s="0" t="n">
+        <f aca="false">Q48/V48</f>
+        <v>0.666597137014315</v>
+      </c>
+      <c r="T48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V48" s="9" t="n">
+        <v>0.489</v>
+      </c>
+      <c r="W48" s="24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>20191028</v>
+      </c>
+      <c r="J52" s="9" t="n">
+        <v>0.388993</v>
+      </c>
+      <c r="K52" s="21" t="n">
+        <v>0.369708</v>
+      </c>
+      <c r="L52" s="9" t="n">
+        <v>0.128825</v>
+      </c>
+      <c r="M52" s="9" t="n">
+        <v>0.358222</v>
+      </c>
+      <c r="N52" s="21" t="n">
+        <v>0.356647</v>
+      </c>
+      <c r="O52" s="9" t="n">
+        <v>0.127494</v>
+      </c>
+      <c r="P52" s="9" t="n">
+        <v>0.333846</v>
+      </c>
+      <c r="Q52" s="21" t="n">
+        <v>0.354364</v>
+      </c>
+      <c r="R52" s="9" t="n">
+        <v>0.127273</v>
+      </c>
+      <c r="S52" s="8" t="n">
+        <f aca="false">Q52/V52</f>
+        <v>0.782087839329066</v>
+      </c>
+      <c r="T52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U52" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V52" s="9" t="n">
+        <v>0.4531</v>
+      </c>
+      <c r="W52" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F56" s="3" t="n">
+        <v>20191028</v>
+      </c>
+      <c r="J56" s="9" t="n">
+        <v>0.342703</v>
+      </c>
+      <c r="K56" s="21" t="n">
+        <v>0.376731</v>
+      </c>
+      <c r="L56" s="9" t="n">
+        <v>0.146181</v>
+      </c>
+      <c r="M56" s="9" t="n">
+        <v>0.185744</v>
+      </c>
+      <c r="N56" s="21" t="n">
+        <v>0.26551</v>
+      </c>
+      <c r="O56" s="9" t="n">
+        <v>0.098929</v>
+      </c>
+      <c r="P56" s="9" t="n">
+        <v>0.111736</v>
+      </c>
+      <c r="Q56" s="21" t="n">
+        <v>0.234004</v>
+      </c>
+      <c r="R56" s="9" t="n">
+        <v>0.084511</v>
+      </c>
+      <c r="S56" s="0" t="n">
+        <f aca="false">Q56/V56</f>
+        <v>0.421097714594205</v>
+      </c>
+      <c r="T56" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="U56" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V56" s="9" t="n">
+        <v>0.5557</v>
+      </c>
+      <c r="W56" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="X56" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="J58" s="9" t="n">
+        <v>0.294119</v>
+      </c>
+      <c r="K58" s="22" t="n">
+        <v>0.393724</v>
+      </c>
+      <c r="L58" s="9" t="n">
+        <v>0.14922</v>
+      </c>
+      <c r="M58" s="9" t="n">
+        <v>0.294119</v>
+      </c>
+      <c r="N58" s="22" t="n">
+        <v>0.393724</v>
+      </c>
+      <c r="O58" s="9" t="n">
+        <v>0.14922</v>
+      </c>
+      <c r="P58" s="9" t="n">
+        <v>0.18846</v>
+      </c>
+      <c r="Q58" s="22" t="n">
+        <v>0.378332</v>
+      </c>
+      <c r="R58" s="9" t="n">
+        <v>0.13538</v>
+      </c>
+      <c r="V58" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="3" t="n">
-        <v>20191028</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="H32" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="J32" s="9" t="n">
-        <v>0.322902</v>
-      </c>
-      <c r="K32" s="20" t="n">
-        <v>0.375154</v>
-      </c>
-      <c r="L32" s="9" t="n">
-        <v>0.144468</v>
-      </c>
-      <c r="M32" s="9" t="n">
-        <v>0.299865</v>
-      </c>
-      <c r="N32" s="21" t="n">
-        <v>0.334215</v>
-      </c>
-      <c r="O32" s="9" t="n">
-        <v>0.128337</v>
-      </c>
-      <c r="P32" s="9" t="n">
-        <v>0.265335</v>
-      </c>
-      <c r="Q32" s="9" t="n">
-        <v>0.325966</v>
-      </c>
-      <c r="R32" s="9" t="n">
-        <v>0.124625</v>
-      </c>
-      <c r="S32" s="0" t="n">
-        <f aca="false">Q32/V32</f>
-        <v>0.666597137014315</v>
-      </c>
-      <c r="T32" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="U32" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="V32" s="9" t="n">
-        <v>0.489</v>
-      </c>
-      <c r="W32" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="3" t="n">
-        <v>20191028</v>
-      </c>
-      <c r="J36" s="9" t="n">
-        <v>0.388993</v>
-      </c>
-      <c r="K36" s="19" t="n">
-        <v>0.369708</v>
-      </c>
-      <c r="L36" s="9" t="n">
-        <v>0.128825</v>
-      </c>
-      <c r="M36" s="9" t="n">
-        <v>0.358222</v>
-      </c>
-      <c r="N36" s="19" t="n">
-        <v>0.356647</v>
-      </c>
-      <c r="O36" s="9" t="n">
-        <v>0.127494</v>
-      </c>
-      <c r="P36" s="9" t="n">
-        <v>0.333846</v>
-      </c>
-      <c r="Q36" s="19" t="n">
-        <v>0.354364</v>
-      </c>
-      <c r="R36" s="9" t="n">
-        <v>0.127273</v>
-      </c>
-      <c r="S36" s="8" t="n">
-        <f aca="false">Q36/V36</f>
-        <v>0.782087839329066</v>
-      </c>
-      <c r="T36" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="U36" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="V36" s="9" t="n">
-        <v>0.4531</v>
-      </c>
-      <c r="W36" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F40" s="3" t="n">
-        <v>20191028</v>
-      </c>
-      <c r="J40" s="9" t="n">
-        <v>0.342703</v>
-      </c>
-      <c r="K40" s="19" t="n">
-        <v>0.376731</v>
-      </c>
-      <c r="L40" s="9" t="n">
-        <v>0.146181</v>
-      </c>
-      <c r="M40" s="9" t="n">
-        <v>0.185744</v>
-      </c>
-      <c r="N40" s="19" t="n">
-        <v>0.26551</v>
-      </c>
-      <c r="O40" s="9" t="n">
-        <v>0.098929</v>
-      </c>
-      <c r="P40" s="9" t="n">
-        <v>0.111736</v>
-      </c>
-      <c r="Q40" s="19" t="n">
-        <v>0.234004</v>
-      </c>
-      <c r="R40" s="9" t="n">
-        <v>0.084511</v>
-      </c>
-      <c r="S40" s="0" t="n">
-        <f aca="false">Q40/V40</f>
-        <v>0.421097714594205</v>
-      </c>
-      <c r="T40" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="U40" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="V40" s="9" t="n">
-        <v>0.5557</v>
-      </c>
-      <c r="W40" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="J47" s="9" t="n">
-        <v>0.570309</v>
-      </c>
-      <c r="K47" s="9" t="n">
-        <v>0.506601</v>
-      </c>
-      <c r="L47" s="9" t="n">
-        <v>0.174945</v>
-      </c>
-      <c r="M47" s="9" t="n">
-        <v>0.497265</v>
-      </c>
-      <c r="N47" s="9" t="n">
-        <v>0.492078</v>
-      </c>
-      <c r="O47" s="9" t="n">
-        <v>0.172062</v>
-      </c>
-      <c r="P47" s="9" t="n">
-        <v>0.517553</v>
-      </c>
-      <c r="Q47" s="9" t="n">
-        <v>0.489173</v>
-      </c>
-      <c r="R47" s="9" t="n">
-        <v>0.173171</v>
-      </c>
-      <c r="W47" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V48" s="2"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="J49" s="9" t="n">
-        <v>0.53527</v>
-      </c>
-      <c r="K49" s="9" t="n">
-        <v>0.624088</v>
-      </c>
-      <c r="L49" s="9" t="n">
-        <v>0.179823</v>
-      </c>
-      <c r="V49" s="2"/>
-      <c r="W49" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V50" s="2"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J51" s="9" t="n">
-        <v>0.509545</v>
-      </c>
-      <c r="K51" s="9" t="n">
-        <v>0.504833</v>
-      </c>
-      <c r="L51" s="9" t="n">
-        <v>0.173614</v>
-      </c>
-      <c r="M51" s="9" t="n">
-        <v>0.334369</v>
-      </c>
-      <c r="N51" s="9" t="n">
-        <v>0.414619</v>
-      </c>
-      <c r="O51" s="9" t="n">
-        <v>0.142572</v>
-      </c>
-      <c r="P51" s="9" t="n">
-        <v>0.260693</v>
-      </c>
-      <c r="Q51" s="23" t="n">
-        <v>0.42473</v>
-      </c>
-      <c r="R51" s="9" t="n">
-        <v>0.137916</v>
-      </c>
-      <c r="S51" s="17" t="n">
-        <f aca="false">Q51/V51</f>
-        <v>0.766245715316616</v>
-      </c>
-      <c r="T51" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="U51" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="V51" s="9" t="n">
-        <v>0.5543</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V52" s="2"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="V53" s="2"/>
-      <c r="W53" s="22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V54" s="2"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J55" s="9" t="n">
-        <v>0.546447</v>
-      </c>
-      <c r="K55" s="9" t="n">
-        <v>0.549731</v>
-      </c>
-      <c r="L55" s="9" t="n">
-        <v>0.196452</v>
-      </c>
-      <c r="M55" s="9" t="n">
-        <v>0.493894</v>
-      </c>
-      <c r="N55" s="9" t="n">
-        <v>0.51285</v>
-      </c>
-      <c r="O55" s="9" t="n">
-        <v>0.180044</v>
-      </c>
-      <c r="P55" s="9" t="n">
-        <v>0.458191</v>
-      </c>
-      <c r="Q55" s="9" t="n">
-        <v>0.490952</v>
-      </c>
-      <c r="R55" s="9" t="n">
-        <v>0.172949</v>
-      </c>
-      <c r="W55" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
+      <c r="W58" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="J60" s="9" t="n">
+        <v>0.382297</v>
+      </c>
+      <c r="K60" s="9" t="n">
+        <v>0.37999</v>
+      </c>
+      <c r="L60" s="9" t="n">
+        <v>0.142206</v>
+      </c>
+      <c r="M60" s="9" t="n">
+        <v>0.257935</v>
+      </c>
+      <c r="N60" s="9" t="n">
+        <v>0.320515</v>
+      </c>
+      <c r="O60" s="9" t="n">
+        <v>0.119599</v>
+      </c>
+      <c r="P60" s="9" t="n">
+        <v>0.174454</v>
+      </c>
+      <c r="Q60" s="21" t="n">
+        <v>0.300714</v>
+      </c>
+      <c r="R60" s="9" t="n">
+        <v>0.109389</v>
+      </c>
+      <c r="V60" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="W60" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="J62" s="9" t="n">
+        <v>0.389024</v>
+      </c>
+      <c r="K62" s="21" t="n">
+        <v>0.363357</v>
+      </c>
+      <c r="L62" s="9" t="n">
+        <v>0.136881</v>
+      </c>
+      <c r="M62" s="9" t="n">
+        <v>0.2268</v>
+      </c>
+      <c r="N62" s="23" t="n">
+        <v>0.282939</v>
+      </c>
+      <c r="O62" s="9" t="n">
+        <v>0.100741</v>
+      </c>
+      <c r="P62" s="9" t="n">
+        <v>0.123446</v>
+      </c>
+      <c r="Q62" s="23" t="n">
+        <v>0.240285</v>
+      </c>
+      <c r="R62" s="9" t="n">
+        <v>0.080884</v>
+      </c>
+      <c r="S62" s="0" t="n">
+        <f aca="false">Q62/V62</f>
+        <v>0.445302075611564</v>
+      </c>
+      <c r="U62" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="V62" s="26" t="n">
+        <v>0.5396</v>
+      </c>
+      <c r="W62" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="X62" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J57" s="9" t="n">
-        <v>0.525183</v>
-      </c>
-      <c r="K57" s="9" t="n">
-        <v>0.539951</v>
-      </c>
-      <c r="L57" s="9" t="n">
-        <v>0.197561</v>
-      </c>
-      <c r="M57" s="9" t="n">
-        <v>0.46354</v>
-      </c>
-      <c r="N57" s="9" t="n">
-        <v>0.48907</v>
-      </c>
-      <c r="O57" s="9" t="n">
-        <v>0.171397</v>
-      </c>
-      <c r="P57" s="9" t="n">
-        <v>0.334369</v>
-      </c>
-      <c r="Q57" s="23" t="n">
-        <v>0.414619</v>
-      </c>
-      <c r="R57" s="9" t="n">
-        <v>0.142572</v>
-      </c>
-      <c r="S57" s="0" t="n">
-        <f aca="false">Q57/V57</f>
-        <v>0.656874207858048</v>
-      </c>
-      <c r="T57" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="U57" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="V57" s="9" t="n">
-        <v>0.6312</v>
-      </c>
-      <c r="W57" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F59" s="3" t="n">
-        <v>20191030</v>
-      </c>
-      <c r="H59" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="J59" s="9" t="n">
-        <v>0.394624</v>
-      </c>
-      <c r="K59" s="9" t="n">
-        <v>0.390665</v>
-      </c>
-      <c r="L59" s="9" t="n">
-        <v>0.13969</v>
-      </c>
-      <c r="M59" s="9" t="n">
-        <v>0.356773</v>
-      </c>
-      <c r="N59" s="9" t="n">
-        <v>0.377995</v>
-      </c>
-      <c r="O59" s="9" t="n">
-        <v>0.136364</v>
-      </c>
-      <c r="P59" s="9" t="n">
-        <v>0.301481</v>
-      </c>
-      <c r="Q59" s="19" t="n">
-        <v>0.383617</v>
-      </c>
-      <c r="R59" s="9" t="n">
-        <v>0.136364</v>
-      </c>
-      <c r="S59" s="8" t="n">
-        <f aca="false">Q59/V59</f>
-        <v>0.775453810390135</v>
-      </c>
-      <c r="T59" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="U59" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="V59" s="9" t="n">
-        <v>0.4947</v>
-      </c>
-      <c r="W59" s="0" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="J61" s="9" t="n">
-        <v>0.155699</v>
-      </c>
-      <c r="K61" s="9" t="n">
-        <v>0.429368</v>
-      </c>
-      <c r="L61" s="9" t="n">
-        <v>0.146785</v>
-      </c>
-      <c r="M61" s="9" t="n">
-        <v>0.14578</v>
-      </c>
-      <c r="N61" s="9" t="n">
-        <v>0.405742</v>
-      </c>
-      <c r="O61" s="9" t="n">
-        <v>0.136585</v>
-      </c>
-      <c r="P61" s="9" t="n">
-        <v>0.139775</v>
-      </c>
-      <c r="Q61" s="9" t="n">
-        <v>0.396125</v>
-      </c>
-      <c r="R61" s="9" t="n">
-        <v>0.133703</v>
-      </c>
-      <c r="U61" s="24" t="n">
-        <v>13</v>
-      </c>
-      <c r="V61" s="25" t="n">
-        <v>0.5043</v>
-      </c>
-      <c r="W61" s="24" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="X61" s="24"/>
-      <c r="Y61" s="24"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="J64" s="9" t="n">
+        <v>0.366225</v>
+      </c>
+      <c r="K64" s="27" t="n">
+        <v>0.399947</v>
+      </c>
+      <c r="L64" s="9" t="n">
+        <v>0.144707</v>
+      </c>
+      <c r="M64" s="9" t="n">
+        <v>0.232135</v>
+      </c>
+      <c r="N64" s="21" t="n">
+        <v>0.335551</v>
+      </c>
+      <c r="O64" s="9" t="n">
+        <v>0.119383</v>
+      </c>
+      <c r="P64" s="9" t="n">
+        <v>0.144385</v>
+      </c>
+      <c r="Q64" s="21" t="n">
+        <v>0.335953</v>
+      </c>
+      <c r="R64" s="9" t="n">
+        <v>0.112338</v>
+      </c>
+      <c r="S64" s="0" t="n">
+        <f aca="false">Q64/V64</f>
+        <v>0.72123872906827</v>
+      </c>
+      <c r="U64" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="V64" s="9" t="n">
+        <v>0.4658</v>
+      </c>
+      <c r="W64" s="0" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="0" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J66" s="9" t="n">
+        <v>0.406997</v>
+      </c>
+      <c r="K66" s="9" t="n">
+        <v>0.413022</v>
+      </c>
+      <c r="L66" s="9" t="n">
+        <v>0.150288</v>
+      </c>
+      <c r="P66" s="9" t="n">
+        <v>0.17971</v>
+      </c>
+      <c r="Q66" s="9" t="n">
+        <v>0.359421</v>
+      </c>
+      <c r="R66" s="9" t="n">
+        <v>0.120326</v>
+      </c>
+      <c r="S66" s="0" t="n">
+        <f aca="false">Q66/V66</f>
+        <v>0.772284056725397</v>
+      </c>
       <c r="U66" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="V66" s="26" t="n">
-        <v>0.4306</v>
+        <v>19</v>
+      </c>
+      <c r="V66" s="9" t="n">
+        <v>0.4654</v>
       </c>
       <c r="W66" s="0" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="J72" s="9" t="n">
+        <v>0.570309</v>
+      </c>
+      <c r="K72" s="9" t="n">
+        <v>0.506601</v>
+      </c>
+      <c r="L72" s="9" t="n">
+        <v>0.174945</v>
+      </c>
+      <c r="M72" s="9" t="n">
+        <v>0.497265</v>
+      </c>
+      <c r="N72" s="9" t="n">
+        <v>0.492078</v>
+      </c>
+      <c r="O72" s="9" t="n">
+        <v>0.172062</v>
+      </c>
+      <c r="P72" s="9" t="n">
+        <v>0.517553</v>
+      </c>
+      <c r="Q72" s="9" t="n">
+        <v>0.489173</v>
+      </c>
+      <c r="R72" s="9" t="n">
+        <v>0.173171</v>
+      </c>
+      <c r="W72" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V73" s="2"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="J74" s="9" t="n">
+        <v>0.53527</v>
+      </c>
+      <c r="K74" s="9" t="n">
+        <v>0.624088</v>
+      </c>
+      <c r="L74" s="9" t="n">
+        <v>0.179823</v>
+      </c>
+      <c r="V74" s="2"/>
+      <c r="W74" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V75" s="2"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J76" s="9" t="n">
+        <v>0.509545</v>
+      </c>
+      <c r="K76" s="9" t="n">
+        <v>0.504833</v>
+      </c>
+      <c r="L76" s="9" t="n">
+        <v>0.173614</v>
+      </c>
+      <c r="M76" s="9" t="n">
+        <v>0.334369</v>
+      </c>
+      <c r="N76" s="9" t="n">
+        <v>0.414619</v>
+      </c>
+      <c r="O76" s="9" t="n">
+        <v>0.142572</v>
+      </c>
+      <c r="P76" s="9" t="n">
+        <v>0.260693</v>
+      </c>
+      <c r="Q76" s="29" t="n">
+        <v>0.42473</v>
+      </c>
+      <c r="R76" s="9" t="n">
+        <v>0.137916</v>
+      </c>
+      <c r="S76" s="15" t="n">
+        <f aca="false">Q76/V76</f>
+        <v>0.766245715316616</v>
+      </c>
+      <c r="T76" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U76" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V76" s="9" t="n">
+        <v>0.5543</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V77" s="2"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="V78" s="2"/>
+      <c r="W78" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V79" s="2"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J80" s="9" t="n">
+        <v>0.546447</v>
+      </c>
+      <c r="K80" s="9" t="n">
+        <v>0.549731</v>
+      </c>
+      <c r="L80" s="9" t="n">
+        <v>0.196452</v>
+      </c>
+      <c r="M80" s="9" t="n">
+        <v>0.493894</v>
+      </c>
+      <c r="N80" s="9" t="n">
+        <v>0.51285</v>
+      </c>
+      <c r="O80" s="9" t="n">
+        <v>0.180044</v>
+      </c>
+      <c r="P80" s="9" t="n">
+        <v>0.458191</v>
+      </c>
+      <c r="Q80" s="9" t="n">
+        <v>0.490952</v>
+      </c>
+      <c r="R80" s="9" t="n">
+        <v>0.172949</v>
+      </c>
+      <c r="W80" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J82" s="9" t="n">
+        <v>0.525183</v>
+      </c>
+      <c r="K82" s="9" t="n">
+        <v>0.539951</v>
+      </c>
+      <c r="L82" s="9" t="n">
+        <v>0.197561</v>
+      </c>
+      <c r="M82" s="9" t="n">
+        <v>0.46354</v>
+      </c>
+      <c r="N82" s="9" t="n">
+        <v>0.48907</v>
+      </c>
+      <c r="O82" s="9" t="n">
+        <v>0.171397</v>
+      </c>
+      <c r="P82" s="9" t="n">
+        <v>0.334369</v>
+      </c>
+      <c r="Q82" s="29" t="n">
+        <v>0.414619</v>
+      </c>
+      <c r="R82" s="9" t="n">
+        <v>0.142572</v>
+      </c>
+      <c r="S82" s="0" t="n">
+        <f aca="false">Q82/V82</f>
+        <v>0.656874207858048</v>
+      </c>
+      <c r="T82" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="U82" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V82" s="9" t="n">
+        <v>0.6312</v>
+      </c>
+      <c r="W82" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F84" s="3" t="n">
+        <v>20191030</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="J84" s="9" t="n">
+        <v>0.394624</v>
+      </c>
+      <c r="K84" s="9" t="n">
+        <v>0.390665</v>
+      </c>
+      <c r="L84" s="9" t="n">
+        <v>0.13969</v>
+      </c>
+      <c r="M84" s="9" t="n">
+        <v>0.356773</v>
+      </c>
+      <c r="N84" s="9" t="n">
+        <v>0.377995</v>
+      </c>
+      <c r="O84" s="9" t="n">
+        <v>0.136364</v>
+      </c>
+      <c r="P84" s="9" t="n">
+        <v>0.301481</v>
+      </c>
+      <c r="Q84" s="21" t="n">
+        <v>0.383617</v>
+      </c>
+      <c r="R84" s="9" t="n">
+        <v>0.136364</v>
+      </c>
+      <c r="S84" s="8" t="n">
+        <f aca="false">Q84/V84</f>
+        <v>0.775453810390135</v>
+      </c>
+      <c r="T84" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U84" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="V84" s="9" t="n">
+        <v>0.4947</v>
+      </c>
+      <c r="W84" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="J86" s="9" t="n">
+        <v>0.155699</v>
+      </c>
+      <c r="K86" s="9" t="n">
+        <v>0.429368</v>
+      </c>
+      <c r="L86" s="9" t="n">
+        <v>0.146785</v>
+      </c>
+      <c r="M86" s="9" t="n">
+        <v>0.14578</v>
+      </c>
+      <c r="N86" s="9" t="n">
+        <v>0.405742</v>
+      </c>
+      <c r="O86" s="9" t="n">
+        <v>0.136585</v>
+      </c>
+      <c r="P86" s="9" t="n">
+        <v>0.139775</v>
+      </c>
+      <c r="Q86" s="9" t="n">
+        <v>0.396125</v>
+      </c>
+      <c r="R86" s="9" t="n">
+        <v>0.133703</v>
+      </c>
+      <c r="U86" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="V86" s="9" t="n">
+        <v>0.5043</v>
+      </c>
+      <c r="W86" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="X86" s="2"/>
+      <c r="Y86" s="2"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="W88" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U93" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="V93" s="31" t="n">
+        <v>0.4306</v>
+      </c>
+      <c r="W93" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="W98" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="W102" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2789,17 +3308,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2810,204 +3329,230 @@
       <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>110</v>
+      <c r="A3" s="32" t="s">
+        <v>143</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C3" s="27" t="n">
+      <c r="C3" s="0" t="n">
         <v>0.4306</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>112</v>
+        <v>144</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="n">
+      <c r="C4" s="9" t="n">
         <v>0.4461</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>114</v>
+        <v>147</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28" t="s">
-        <v>79</v>
+      <c r="A5" s="32" t="s">
+        <v>93</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="25" t="n">
+      <c r="C5" s="9" t="n">
         <v>0.4531</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>114</v>
+        <v>149</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>0.4849</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="25" t="n">
+      <c r="C7" s="9" t="n">
         <v>0.489</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="E7" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C7" s="25" t="n">
+      <c r="C8" s="9" t="n">
         <v>0.4947</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="D8" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C8" s="25" t="n">
+      <c r="C9" s="9" t="n">
         <v>0.4988</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G9" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9" t="n">
+        <v>0.5043</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9" t="n">
+        <v>0.5215</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9" t="n">
+        <v>0.5543</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="24" t="n">
-        <v>13</v>
-      </c>
-      <c r="C9" s="25" t="n">
-        <v>0.5043</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="0" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="n">
+        <v>0.5557</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C14" s="9" t="n">
+        <v>0.6312</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="25" t="n">
-        <v>0.5215</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C11" s="25" t="n">
-        <v>0.5543</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="25" t="n">
-        <v>0.5557</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C13" s="25" t="n">
-        <v>0.6312</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>100</v>
+      <c r="G14" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3098,4 +3643,88 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Efficientnet, Densenet, resnet large
</commit_message>
<xml_diff>
--- a/model_metrics.xlsx
+++ b/model_metrics.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="187">
   <si>
     <t xml:space="preserve">nb</t>
   </si>
@@ -262,6 +262,48 @@
     <t xml:space="preserve">03_18</t>
   </si>
   <si>
+    <t xml:space="preserve">xtra_tfms=[dihedral(p=0.7), rand_crop(p=0.4)], (flip_vert=True, max_lighting=0.2, max_zoom=1.1, max_warp=0., xtra_tfms=xtra_tfms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As 03_11 (valid only), using 4x4 bg padded, wrap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generated sub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padded bg, 256 then 512 img size, resnet 50, 101, 152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_20_fastai_train_resnet_valid_pad_refl_20191118.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As 03_11 (valid only), using 4x4 bg padded, reflect, 256 then 512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rn101-03_21-cv_reflect_101_valid-20191118-7607ef2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As 03_20 but resnet101, extra tfms (with 256 then 512)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generated sub on 2 (not 2-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_22_fastai_train_resnet152_valid_pad_refl_20191118.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As 03_20 but resnet152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO – train on full non clipped bg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Using sharpend images</t>
   </si>
   <si>
@@ -425,6 +467,18 @@
   </si>
   <si>
     <t xml:space="preserve">strted looking at this buty fair bit of work to get training then more work to get pred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06_9_fastai_train_efficientnet_b3_20191117.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">efficientnet_b3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06_10_fastai_train_efficientnet_b6_20191117.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">efficientnet_b6</t>
   </si>
   <si>
     <t xml:space="preserve">Ensembles</t>
@@ -581,15 +635,15 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="21">
@@ -748,7 +802,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -829,6 +883,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -853,7 +919,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -874,10 +940,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -969,7 +1031,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1103,11 +1165,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9835685"/>
-        <c:axId val="48529175"/>
+        <c:axId val="52458119"/>
+        <c:axId val="61791446"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9835685"/>
+        <c:axId val="52458119"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,12 +1197,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48529175"/>
+        <c:crossAx val="61791446"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48529175"/>
+        <c:axId val="61791446"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1177,7 +1239,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9835685"/>
+        <c:crossAx val="52458119"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1225,7 +1287,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1349,11 +1411,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="22864067"/>
-        <c:axId val="91927152"/>
+        <c:axId val="72555897"/>
+        <c:axId val="60811836"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="22864067"/>
+        <c:axId val="72555897"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,14 +1443,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91927152"/>
+        <c:crossAx val="60811836"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91927152"/>
+        <c:axId val="60811836"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1487,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22864067"/>
+        <c:crossAx val="72555897"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1472,7 +1534,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1563,11 +1625,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="93109884"/>
-        <c:axId val="71181858"/>
+        <c:axId val="9619229"/>
+        <c:axId val="13932766"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93109884"/>
+        <c:axId val="9619229"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1595,14 +1657,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71181858"/>
+        <c:crossAx val="13932766"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71181858"/>
+        <c:axId val="13932766"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -1640,7 +1702,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93109884"/>
+        <c:crossAx val="9619229"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1699,9 +1761,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>38880</xdr:colOff>
+      <xdr:colOff>38520</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1710,7 +1772,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9865800" y="2483640"/>
-        <a:ext cx="5757840" cy="3237840"/>
+        <a:ext cx="5757480" cy="3237480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1729,9 +1791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>300240</xdr:colOff>
+      <xdr:colOff>299880</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1740,7 +1802,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="118800" y="2572200"/>
-        <a:ext cx="9263520" cy="3240000"/>
+        <a:ext cx="9263160" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1764,9 +1826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>156240</xdr:colOff>
+      <xdr:colOff>155880</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1775,7 +1837,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1714680" y="2696400"/>
-        <a:ext cx="5756760" cy="3239640"/>
+        <a:ext cx="5756400" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1793,10 +1855,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y102"/>
+  <dimension ref="A1:Y113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W39" activeCellId="0" sqref="W39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2440,856 +2502,976 @@
       <c r="B39" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="V39" s="0" t="n">
+      <c r="V39" s="15" t="n">
         <v>0.4535</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="W39" s="0" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="W40" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="X40" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P43" s="9" t="n">
+        <v>0.473367</v>
+      </c>
+      <c r="Q43" s="9" t="n">
+        <v>0.488676</v>
+      </c>
+      <c r="R43" s="9" t="n">
+        <v>0.176866</v>
+      </c>
+      <c r="V43" s="9" t="n">
+        <v>0.4629</v>
+      </c>
+      <c r="W43" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="X43" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J44" s="9" t="n">
+        <v>0.518463</v>
+      </c>
+      <c r="K44" s="9" t="n">
+        <v>0.543399</v>
+      </c>
+      <c r="L44" s="9" t="n">
+        <v>0.201076</v>
+      </c>
+      <c r="M44" s="9" t="n">
+        <v>0.351982</v>
+      </c>
+      <c r="N44" s="9" t="n">
+        <v>0.506825</v>
+      </c>
+      <c r="O44" s="9" t="n">
+        <v>0.178211</v>
+      </c>
+      <c r="V44" s="9" t="n">
+        <v>0.5733</v>
+      </c>
+      <c r="W44" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="X44" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="M45" s="9" t="n">
+        <v>0.427257</v>
+      </c>
+      <c r="N45" s="9" t="n">
+        <v>0.50657</v>
+      </c>
+      <c r="O45" s="9" t="n">
+        <v>0.17384</v>
+      </c>
+      <c r="P45" s="2"/>
+      <c r="W45" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="2"/>
+      <c r="W46" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F43" s="3" t="n">
+      <c r="D50" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F50" s="3" t="n">
         <v>20191027</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H43" s="0" t="n">
+      <c r="G50" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H50" s="0" t="n">
         <v>256</v>
       </c>
-      <c r="I43" s="0" t="s">
+      <c r="I50" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="J43" s="9" t="n">
+      <c r="J50" s="9" t="n">
         <v>0.371694</v>
       </c>
-      <c r="K43" s="20" t="n">
+      <c r="K50" s="23" t="n">
         <v>0.366708</v>
       </c>
-      <c r="L43" s="9" t="n">
+      <c r="L50" s="9" t="n">
         <v>0.129712</v>
       </c>
-      <c r="M43" s="9" t="n">
+      <c r="M50" s="9" t="n">
         <v>0.351872</v>
       </c>
-      <c r="N43" s="21" t="n">
+      <c r="N50" s="24" t="n">
         <v>0.355532</v>
       </c>
-      <c r="O43" s="9" t="n">
+      <c r="O50" s="9" t="n">
         <v>0.127273</v>
       </c>
-      <c r="U43" s="0" t="n">
+      <c r="U50" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="V43" s="9" t="n">
+      <c r="V50" s="9" t="n">
         <v>0.4916</v>
       </c>
-      <c r="W43" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="W50" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="F48" s="3" t="n">
+      <c r="D55" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F55" s="3" t="n">
         <v>20191028</v>
       </c>
-      <c r="G48" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H48" s="0" t="n">
+      <c r="G55" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55" s="0" t="n">
         <v>256</v>
       </c>
-      <c r="J48" s="9" t="n">
+      <c r="J55" s="9" t="n">
         <v>0.322902</v>
       </c>
-      <c r="K48" s="22" t="n">
+      <c r="K55" s="25" t="n">
         <v>0.375154</v>
       </c>
-      <c r="L48" s="9" t="n">
+      <c r="L55" s="9" t="n">
         <v>0.144468</v>
       </c>
-      <c r="M48" s="9" t="n">
+      <c r="M55" s="9" t="n">
         <v>0.299865</v>
       </c>
-      <c r="N48" s="23" t="n">
+      <c r="N55" s="26" t="n">
         <v>0.334215</v>
       </c>
-      <c r="O48" s="9" t="n">
+      <c r="O55" s="9" t="n">
         <v>0.128337</v>
       </c>
-      <c r="P48" s="9" t="n">
+      <c r="P55" s="9" t="n">
         <v>0.265335</v>
       </c>
-      <c r="Q48" s="9" t="n">
+      <c r="Q55" s="9" t="n">
         <v>0.325966</v>
       </c>
-      <c r="R48" s="9" t="n">
+      <c r="R55" s="9" t="n">
         <v>0.124625</v>
       </c>
-      <c r="S48" s="0" t="n">
-        <f aca="false">Q48/V48</f>
+      <c r="S55" s="0" t="n">
+        <f aca="false">Q55/V55</f>
         <v>0.666597137014315</v>
       </c>
-      <c r="T48" s="0" t="n">
+      <c r="T55" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="U48" s="0" t="n">
+      <c r="U55" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="V48" s="9" t="n">
+      <c r="V55" s="9" t="n">
         <v>0.489</v>
       </c>
-      <c r="W48" s="24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="W55" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="F52" s="3" t="n">
+      <c r="D59" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F59" s="3" t="n">
         <v>20191028</v>
       </c>
-      <c r="J52" s="9" t="n">
+      <c r="J59" s="9" t="n">
         <v>0.388993</v>
       </c>
-      <c r="K52" s="21" t="n">
+      <c r="K59" s="24" t="n">
         <v>0.369708</v>
       </c>
-      <c r="L52" s="9" t="n">
+      <c r="L59" s="9" t="n">
         <v>0.128825</v>
       </c>
-      <c r="M52" s="9" t="n">
+      <c r="M59" s="9" t="n">
         <v>0.358222</v>
       </c>
-      <c r="N52" s="21" t="n">
+      <c r="N59" s="24" t="n">
         <v>0.356647</v>
       </c>
-      <c r="O52" s="9" t="n">
+      <c r="O59" s="9" t="n">
         <v>0.127494</v>
       </c>
-      <c r="P52" s="9" t="n">
+      <c r="P59" s="9" t="n">
         <v>0.333846</v>
       </c>
-      <c r="Q52" s="21" t="n">
+      <c r="Q59" s="24" t="n">
         <v>0.354364</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="R59" s="9" t="n">
         <v>0.127273</v>
       </c>
-      <c r="S52" s="8" t="n">
-        <f aca="false">Q52/V52</f>
+      <c r="S59" s="8" t="n">
+        <f aca="false">Q59/V59</f>
         <v>0.782087839329066</v>
       </c>
-      <c r="T52" s="0" t="n">
+      <c r="T59" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="U52" s="0" t="n">
+      <c r="U59" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="V52" s="9" t="n">
+      <c r="V59" s="9" t="n">
         <v>0.4531</v>
       </c>
-      <c r="W52" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="W59" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D63" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E56" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F56" s="3" t="n">
+      <c r="E63" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F63" s="3" t="n">
         <v>20191028</v>
       </c>
-      <c r="J56" s="9" t="n">
+      <c r="J63" s="9" t="n">
         <v>0.342703</v>
       </c>
-      <c r="K56" s="21" t="n">
+      <c r="K63" s="24" t="n">
         <v>0.376731</v>
       </c>
-      <c r="L56" s="9" t="n">
+      <c r="L63" s="9" t="n">
         <v>0.146181</v>
       </c>
-      <c r="M56" s="9" t="n">
+      <c r="M63" s="9" t="n">
         <v>0.185744</v>
       </c>
-      <c r="N56" s="21" t="n">
+      <c r="N63" s="24" t="n">
         <v>0.26551</v>
       </c>
-      <c r="O56" s="9" t="n">
+      <c r="O63" s="9" t="n">
         <v>0.098929</v>
       </c>
-      <c r="P56" s="9" t="n">
+      <c r="P63" s="9" t="n">
         <v>0.111736</v>
       </c>
-      <c r="Q56" s="21" t="n">
+      <c r="Q63" s="24" t="n">
         <v>0.234004</v>
       </c>
-      <c r="R56" s="9" t="n">
+      <c r="R63" s="9" t="n">
         <v>0.084511</v>
       </c>
-      <c r="S56" s="0" t="n">
-        <f aca="false">Q56/V56</f>
+      <c r="S63" s="0" t="n">
+        <f aca="false">Q63/V63</f>
         <v>0.421097714594205</v>
       </c>
-      <c r="T56" s="0" t="n">
+      <c r="T63" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="U56" s="0" t="n">
+      <c r="U63" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="V56" s="9" t="n">
+      <c r="V63" s="9" t="n">
         <v>0.5557</v>
       </c>
-      <c r="W56" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="X56" s="25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="J58" s="9" t="n">
+      <c r="W63" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="X63" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J65" s="9" t="n">
         <v>0.294119</v>
       </c>
-      <c r="K58" s="22" t="n">
+      <c r="K65" s="25" t="n">
         <v>0.393724</v>
       </c>
-      <c r="L58" s="9" t="n">
+      <c r="L65" s="9" t="n">
         <v>0.14922</v>
       </c>
-      <c r="M58" s="9" t="n">
+      <c r="M65" s="9" t="n">
         <v>0.294119</v>
       </c>
-      <c r="N58" s="22" t="n">
+      <c r="N65" s="25" t="n">
         <v>0.393724</v>
       </c>
-      <c r="O58" s="9" t="n">
+      <c r="O65" s="9" t="n">
         <v>0.14922</v>
       </c>
-      <c r="P58" s="9" t="n">
+      <c r="P65" s="9" t="n">
         <v>0.18846</v>
       </c>
-      <c r="Q58" s="22" t="n">
+      <c r="Q65" s="25" t="n">
         <v>0.378332</v>
       </c>
-      <c r="R58" s="9" t="n">
+      <c r="R65" s="9" t="n">
         <v>0.13538</v>
       </c>
-      <c r="V58" s="18" t="s">
+      <c r="V65" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="W58" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J60" s="9" t="n">
+      <c r="W65" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J67" s="9" t="n">
         <v>0.382297</v>
       </c>
-      <c r="K60" s="9" t="n">
+      <c r="K67" s="9" t="n">
         <v>0.37999</v>
       </c>
-      <c r="L60" s="9" t="n">
+      <c r="L67" s="9" t="n">
         <v>0.142206</v>
       </c>
-      <c r="M60" s="9" t="n">
+      <c r="M67" s="9" t="n">
         <v>0.257935</v>
       </c>
-      <c r="N60" s="9" t="n">
+      <c r="N67" s="9" t="n">
         <v>0.320515</v>
       </c>
-      <c r="O60" s="9" t="n">
+      <c r="O67" s="9" t="n">
         <v>0.119599</v>
       </c>
-      <c r="P60" s="9" t="n">
+      <c r="P67" s="9" t="n">
         <v>0.174454</v>
       </c>
-      <c r="Q60" s="21" t="n">
+      <c r="Q67" s="24" t="n">
         <v>0.300714</v>
       </c>
-      <c r="R60" s="9" t="n">
+      <c r="R67" s="9" t="n">
         <v>0.109389</v>
       </c>
-      <c r="V60" s="18" t="s">
+      <c r="V67" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="W60" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="J62" s="9" t="n">
+      <c r="W67" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J69" s="9" t="n">
         <v>0.389024</v>
       </c>
-      <c r="K62" s="21" t="n">
+      <c r="K69" s="24" t="n">
         <v>0.363357</v>
       </c>
-      <c r="L62" s="9" t="n">
+      <c r="L69" s="9" t="n">
         <v>0.136881</v>
       </c>
-      <c r="M62" s="9" t="n">
+      <c r="M69" s="9" t="n">
         <v>0.2268</v>
       </c>
-      <c r="N62" s="23" t="n">
+      <c r="N69" s="26" t="n">
         <v>0.282939</v>
       </c>
-      <c r="O62" s="9" t="n">
+      <c r="O69" s="9" t="n">
         <v>0.100741</v>
       </c>
-      <c r="P62" s="9" t="n">
+      <c r="P69" s="9" t="n">
         <v>0.123446</v>
       </c>
-      <c r="Q62" s="23" t="n">
+      <c r="Q69" s="26" t="n">
         <v>0.240285</v>
       </c>
-      <c r="R62" s="9" t="n">
+      <c r="R69" s="9" t="n">
         <v>0.080884</v>
       </c>
-      <c r="S62" s="0" t="n">
-        <f aca="false">Q62/V62</f>
+      <c r="S69" s="0" t="n">
+        <f aca="false">Q69/V69</f>
         <v>0.445302075611564</v>
       </c>
-      <c r="U62" s="0" t="n">
+      <c r="U69" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="V62" s="26" t="n">
+      <c r="V69" s="29" t="n">
         <v>0.5396</v>
       </c>
-      <c r="W62" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="X62" s="25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="J64" s="9" t="n">
+      <c r="W69" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="X69" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J71" s="9" t="n">
         <v>0.366225</v>
       </c>
-      <c r="K64" s="27" t="n">
+      <c r="K71" s="30" t="n">
         <v>0.399947</v>
       </c>
-      <c r="L64" s="9" t="n">
+      <c r="L71" s="9" t="n">
         <v>0.144707</v>
       </c>
-      <c r="M64" s="9" t="n">
+      <c r="M71" s="9" t="n">
         <v>0.232135</v>
       </c>
-      <c r="N64" s="21" t="n">
+      <c r="N71" s="24" t="n">
         <v>0.335551</v>
       </c>
-      <c r="O64" s="9" t="n">
+      <c r="O71" s="9" t="n">
         <v>0.119383</v>
       </c>
-      <c r="P64" s="9" t="n">
+      <c r="P71" s="9" t="n">
         <v>0.144385</v>
       </c>
-      <c r="Q64" s="21" t="n">
+      <c r="Q71" s="24" t="n">
         <v>0.335953</v>
       </c>
-      <c r="R64" s="9" t="n">
+      <c r="R71" s="9" t="n">
         <v>0.112338</v>
       </c>
-      <c r="S64" s="0" t="n">
-        <f aca="false">Q64/V64</f>
+      <c r="S71" s="0" t="n">
+        <f aca="false">Q71/V71</f>
         <v>0.72123872906827</v>
       </c>
-      <c r="U64" s="0" t="n">
+      <c r="U71" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="V64" s="9" t="n">
+      <c r="V71" s="9" t="n">
         <v>0.4658</v>
       </c>
-      <c r="W64" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="J66" s="9" t="n">
+      <c r="W71" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="J73" s="9" t="n">
         <v>0.406997</v>
       </c>
-      <c r="K66" s="9" t="n">
+      <c r="K73" s="9" t="n">
         <v>0.413022</v>
       </c>
-      <c r="L66" s="9" t="n">
+      <c r="L73" s="9" t="n">
         <v>0.150288</v>
       </c>
-      <c r="P66" s="9" t="n">
+      <c r="P73" s="9" t="n">
         <v>0.17971</v>
       </c>
-      <c r="Q66" s="9" t="n">
+      <c r="Q73" s="9" t="n">
         <v>0.359421</v>
       </c>
-      <c r="R66" s="9" t="n">
+      <c r="R73" s="9" t="n">
         <v>0.120326</v>
       </c>
-      <c r="S66" s="0" t="n">
-        <f aca="false">Q66/V66</f>
+      <c r="S73" s="0" t="n">
+        <f aca="false">Q73/V73</f>
         <v>0.772284056725397</v>
       </c>
-      <c r="U66" s="0" t="n">
+      <c r="U73" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="V66" s="9" t="n">
+      <c r="V73" s="9" t="n">
         <v>0.4654</v>
       </c>
-      <c r="W66" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="J72" s="9" t="n">
+      <c r="W73" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="J79" s="9" t="n">
         <v>0.570309</v>
       </c>
-      <c r="K72" s="9" t="n">
+      <c r="K79" s="9" t="n">
         <v>0.506601</v>
       </c>
-      <c r="L72" s="9" t="n">
+      <c r="L79" s="9" t="n">
         <v>0.174945</v>
       </c>
-      <c r="M72" s="9" t="n">
+      <c r="M79" s="9" t="n">
         <v>0.497265</v>
       </c>
-      <c r="N72" s="9" t="n">
+      <c r="N79" s="9" t="n">
         <v>0.492078</v>
       </c>
-      <c r="O72" s="9" t="n">
+      <c r="O79" s="9" t="n">
         <v>0.172062</v>
       </c>
-      <c r="P72" s="9" t="n">
+      <c r="P79" s="9" t="n">
         <v>0.517553</v>
       </c>
-      <c r="Q72" s="9" t="n">
+      <c r="Q79" s="9" t="n">
         <v>0.489173</v>
       </c>
-      <c r="R72" s="9" t="n">
+      <c r="R79" s="9" t="n">
         <v>0.173171</v>
       </c>
-      <c r="W72" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V73" s="2"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="J74" s="9" t="n">
+      <c r="W79" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V80" s="2"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="J81" s="9" t="n">
         <v>0.53527</v>
       </c>
-      <c r="K74" s="9" t="n">
+      <c r="K81" s="9" t="n">
         <v>0.624088</v>
       </c>
-      <c r="L74" s="9" t="n">
+      <c r="L81" s="9" t="n">
         <v>0.179823</v>
       </c>
-      <c r="V74" s="2"/>
-      <c r="W74" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V75" s="2"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="J76" s="9" t="n">
+      <c r="V81" s="2"/>
+      <c r="W81" s="31" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V82" s="2"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J83" s="9" t="n">
         <v>0.509545</v>
       </c>
-      <c r="K76" s="9" t="n">
+      <c r="K83" s="9" t="n">
         <v>0.504833</v>
       </c>
-      <c r="L76" s="9" t="n">
+      <c r="L83" s="9" t="n">
         <v>0.173614</v>
       </c>
-      <c r="M76" s="9" t="n">
+      <c r="M83" s="9" t="n">
         <v>0.334369</v>
       </c>
-      <c r="N76" s="9" t="n">
+      <c r="N83" s="9" t="n">
         <v>0.414619</v>
       </c>
-      <c r="O76" s="9" t="n">
+      <c r="O83" s="9" t="n">
         <v>0.142572</v>
       </c>
-      <c r="P76" s="9" t="n">
+      <c r="P83" s="9" t="n">
         <v>0.260693</v>
       </c>
-      <c r="Q76" s="29" t="n">
+      <c r="Q83" s="32" t="n">
         <v>0.42473</v>
       </c>
-      <c r="R76" s="9" t="n">
+      <c r="R83" s="9" t="n">
         <v>0.137916</v>
       </c>
-      <c r="S76" s="15" t="n">
-        <f aca="false">Q76/V76</f>
+      <c r="S83" s="15" t="n">
+        <f aca="false">Q83/V83</f>
         <v>0.766245715316616</v>
       </c>
-      <c r="T76" s="0" t="n">
+      <c r="T83" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="U76" s="0" t="n">
+      <c r="U83" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="V76" s="9" t="n">
+      <c r="V83" s="9" t="n">
         <v>0.5543</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V77" s="2"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="V78" s="2"/>
-      <c r="W78" s="28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V79" s="2"/>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="J80" s="9" t="n">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V84" s="2"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="V85" s="2"/>
+      <c r="W85" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V86" s="2"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J87" s="9" t="n">
         <v>0.546447</v>
       </c>
-      <c r="K80" s="9" t="n">
+      <c r="K87" s="9" t="n">
         <v>0.549731</v>
       </c>
-      <c r="L80" s="9" t="n">
+      <c r="L87" s="9" t="n">
         <v>0.196452</v>
       </c>
-      <c r="M80" s="9" t="n">
+      <c r="M87" s="9" t="n">
         <v>0.493894</v>
       </c>
-      <c r="N80" s="9" t="n">
+      <c r="N87" s="9" t="n">
         <v>0.51285</v>
       </c>
-      <c r="O80" s="9" t="n">
+      <c r="O87" s="9" t="n">
         <v>0.180044</v>
       </c>
-      <c r="P80" s="9" t="n">
+      <c r="P87" s="9" t="n">
         <v>0.458191</v>
       </c>
-      <c r="Q80" s="9" t="n">
+      <c r="Q87" s="9" t="n">
         <v>0.490952</v>
       </c>
-      <c r="R80" s="9" t="n">
+      <c r="R87" s="9" t="n">
         <v>0.172949</v>
       </c>
-      <c r="W80" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="J82" s="9" t="n">
+      <c r="W87" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J89" s="9" t="n">
         <v>0.525183</v>
       </c>
-      <c r="K82" s="9" t="n">
+      <c r="K89" s="9" t="n">
         <v>0.539951</v>
       </c>
-      <c r="L82" s="9" t="n">
+      <c r="L89" s="9" t="n">
         <v>0.197561</v>
       </c>
-      <c r="M82" s="9" t="n">
+      <c r="M89" s="9" t="n">
         <v>0.46354</v>
       </c>
-      <c r="N82" s="9" t="n">
+      <c r="N89" s="9" t="n">
         <v>0.48907</v>
       </c>
-      <c r="O82" s="9" t="n">
+      <c r="O89" s="9" t="n">
         <v>0.171397</v>
       </c>
-      <c r="P82" s="9" t="n">
+      <c r="P89" s="9" t="n">
         <v>0.334369</v>
       </c>
-      <c r="Q82" s="29" t="n">
+      <c r="Q89" s="32" t="n">
         <v>0.414619</v>
       </c>
-      <c r="R82" s="9" t="n">
+      <c r="R89" s="9" t="n">
         <v>0.142572</v>
       </c>
-      <c r="S82" s="0" t="n">
-        <f aca="false">Q82/V82</f>
+      <c r="S89" s="0" t="n">
+        <f aca="false">Q89/V89</f>
         <v>0.656874207858048</v>
       </c>
-      <c r="T82" s="0" t="n">
+      <c r="T89" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U82" s="0" t="n">
+      <c r="U89" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="V82" s="9" t="n">
+      <c r="V89" s="9" t="n">
         <v>0.6312</v>
       </c>
-      <c r="W82" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D84" s="0" t="s">
+      <c r="W89" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D91" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F84" s="3" t="n">
+      <c r="E91" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F91" s="3" t="n">
         <v>20191030</v>
       </c>
-      <c r="H84" s="0" t="n">
+      <c r="H91" s="0" t="n">
         <v>256</v>
       </c>
-      <c r="J84" s="9" t="n">
+      <c r="J91" s="9" t="n">
         <v>0.394624</v>
       </c>
-      <c r="K84" s="9" t="n">
+      <c r="K91" s="9" t="n">
         <v>0.390665</v>
       </c>
-      <c r="L84" s="9" t="n">
+      <c r="L91" s="9" t="n">
         <v>0.13969</v>
       </c>
-      <c r="M84" s="9" t="n">
+      <c r="M91" s="9" t="n">
         <v>0.356773</v>
       </c>
-      <c r="N84" s="9" t="n">
+      <c r="N91" s="9" t="n">
         <v>0.377995</v>
       </c>
-      <c r="O84" s="9" t="n">
+      <c r="O91" s="9" t="n">
         <v>0.136364</v>
       </c>
-      <c r="P84" s="9" t="n">
+      <c r="P91" s="9" t="n">
         <v>0.301481</v>
       </c>
-      <c r="Q84" s="21" t="n">
+      <c r="Q91" s="24" t="n">
         <v>0.383617</v>
       </c>
-      <c r="R84" s="9" t="n">
+      <c r="R91" s="9" t="n">
         <v>0.136364</v>
       </c>
-      <c r="S84" s="8" t="n">
-        <f aca="false">Q84/V84</f>
+      <c r="S91" s="8" t="n">
+        <f aca="false">Q91/V91</f>
         <v>0.775453810390135</v>
       </c>
-      <c r="T84" s="0" t="n">
+      <c r="T91" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="U84" s="0" t="n">
+      <c r="U91" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="V84" s="9" t="n">
+      <c r="V91" s="9" t="n">
         <v>0.4947</v>
       </c>
-      <c r="W84" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="J86" s="9" t="n">
+      <c r="W91" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="J93" s="9" t="n">
         <v>0.155699</v>
       </c>
-      <c r="K86" s="9" t="n">
+      <c r="K93" s="9" t="n">
         <v>0.429368</v>
       </c>
-      <c r="L86" s="9" t="n">
+      <c r="L93" s="9" t="n">
         <v>0.146785</v>
       </c>
-      <c r="M86" s="9" t="n">
+      <c r="M93" s="9" t="n">
         <v>0.14578</v>
       </c>
-      <c r="N86" s="9" t="n">
+      <c r="N93" s="9" t="n">
         <v>0.405742</v>
       </c>
-      <c r="O86" s="9" t="n">
+      <c r="O93" s="9" t="n">
         <v>0.136585</v>
       </c>
-      <c r="P86" s="9" t="n">
+      <c r="P93" s="9" t="n">
         <v>0.139775</v>
       </c>
-      <c r="Q86" s="9" t="n">
+      <c r="Q93" s="9" t="n">
         <v>0.396125</v>
       </c>
-      <c r="R86" s="9" t="n">
+      <c r="R93" s="9" t="n">
         <v>0.133703</v>
       </c>
-      <c r="U86" s="2" t="n">
+      <c r="U93" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="V86" s="9" t="n">
+      <c r="V93" s="9" t="n">
         <v>0.5043</v>
       </c>
-      <c r="W86" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="X86" s="2"/>
-      <c r="Y86" s="2"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="W88" s="30" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="U93" s="0" t="n">
+      <c r="W93" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="X93" s="2"/>
+      <c r="Y93" s="2"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="W95" s="33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="W97" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="W99" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U104" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="V93" s="31" t="n">
+      <c r="V104" s="34" t="n">
         <v>0.4306</v>
       </c>
-      <c r="W93" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="W98" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="W102" s="0" t="s">
-        <v>141</v>
+      <c r="W104" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="W109" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="W113" s="0" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3333,12 +3515,12 @@
         <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32" t="s">
-        <v>143</v>
+      <c r="A3" s="21" t="s">
+        <v>161</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>11</v>
@@ -3347,14 +3529,14 @@
         <v>0.4306</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -3367,18 +3549,18 @@
         <v>24</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
-        <v>93</v>
+      <c r="A5" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
@@ -3390,14 +3572,14 @@
         <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="35" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="2" t="n">
@@ -3407,18 +3589,18 @@
         <v>0.4849</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="s">
-        <v>88</v>
+      <c r="A7" s="35" t="s">
+        <v>102</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -3430,15 +3612,15 @@
         <v>24</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33" t="s">
-        <v>128</v>
+      <c r="A8" s="35" t="s">
+        <v>142</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>8</v>
@@ -3447,15 +3629,15 @@
         <v>0.4947</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33" t="s">
-        <v>152</v>
+      <c r="A9" s="35" t="s">
+        <v>170</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>9</v>
@@ -3467,12 +3649,12 @@
         <v>24</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="33" t="s">
-        <v>154</v>
+      <c r="A10" s="35" t="s">
+        <v>172</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>13</v>
@@ -3481,15 +3663,15 @@
         <v>0.5043</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
-        <v>155</v>
+      <c r="A11" s="36" t="s">
+        <v>173</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10</v>
@@ -3501,12 +3683,12 @@
         <v>24</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
-        <v>157</v>
+      <c r="A12" s="37" t="s">
+        <v>175</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>6</v>
@@ -3515,12 +3697,12 @@
         <v>0.5543</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
-        <v>97</v>
+      <c r="A13" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -3532,15 +3714,15 @@
         <v>24</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="s">
-        <v>124</v>
+      <c r="A14" s="38" t="s">
+        <v>138</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -3549,10 +3731,10 @@
         <v>0.6312</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3665,57 +3847,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="9" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="9" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="9" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="9" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="9" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="9" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="9" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="9" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="9" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>